<commit_message>
Uploading Time Sheets Nilangi a1882259
Modified Time Sheets
</commit_message>
<xml_diff>
--- a/Project Management/timesheets/MCI-Timesheet - Nilangi - a1882259.xlsx
+++ b/Project Management/timesheets/MCI-Timesheet - Nilangi - a1882259.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MCI_Project\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F37A55-74E4-4DC2-8A28-04F885C361F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331F6787-2F6E-4E58-B781-24EC16A27C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="124">
   <si>
     <t>MCI Project Weekly Time Sheet</t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>Provided advice to others how to start front end development and divided tasks.</t>
+  </si>
+  <si>
+    <t>Prepared business case and draft plan.</t>
+  </si>
+  <si>
+    <t>Completed business case and draft plan.</t>
+  </si>
+  <si>
+    <t>Worked on Business Case and draft plan including Gantt Chart.</t>
   </si>
 </sst>
 </file>
@@ -937,8 +946,8 @@
   </sheetPr>
   <dimension ref="A2:AW72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="82" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2211,13 +2220,13 @@
         <v>45378</v>
       </c>
       <c r="C56" s="13">
-        <v>0.41666666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="D56" s="13">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E56" s="14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>99</v>
@@ -2295,16 +2304,16 @@
         <v>0.5</v>
       </c>
       <c r="E59" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -2313,7 +2322,7 @@
       </c>
       <c r="E60" s="5">
         <f>SUM(E54:E59)</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>